<commit_message>
Cambios hechos durante la call
</commit_message>
<xml_diff>
--- a/datos/Generador inputs horarios.xlsx
+++ b/datos/Generador inputs horarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\practicaevol\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6A4CA8C-4442-4080-8117-0C9F829D8348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241BF4DD-2AEA-4BE9-A30A-788AA5DADD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="I7">
-        <f>IF(H7="","",SUM(D24:AC24))</f>
+        <f t="shared" ref="I7:I19" si="1">IF(H7="","",SUM(D24:AC24))</f>
         <v>18</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -997,18 +997,18 @@
         <v>28</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E10" si="1">SUM(D54:H54)</f>
+        <f t="shared" ref="E8:E10" si="2">SUM(D54:H54)</f>
         <v>29</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ref="F8:F19" si="2">IF(E8&gt;=D8,"OK","ERROR")</f>
+        <f t="shared" ref="F8:F19" si="3">IF(E8&gt;=D8,"OK","ERROR")</f>
         <v>OK</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I8">
-        <f>IF(H8="","",SUM(D25:AC25))</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1035,18 +1035,18 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I9">
-        <f>IF(H9="","",SUM(D26:AC26))</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1066,18 +1066,18 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="I10">
-        <f>IF(H10="","",SUM(D27:AC27))</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1091,14 +1091,10 @@
     <row r="11" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" t="str">
-        <f>IF(H11="","",SUM(D28:AC28))</f>
-        <v/>
-      </c>
       <c r="K11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1110,16 +1106,16 @@
     <row r="12" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" t="str">
-        <f>IF(C12="","",A44)</f>
+        <f t="shared" ref="D12:D19" si="4">IF(C12="","",A44)</f>
         <v/>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" t="str">
-        <f>IF(H12="","",SUM(D29:AC29))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K12" s="2" t="s">
@@ -1133,16 +1129,16 @@
     <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" t="str">
-        <f>IF(C13="","",A45)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" t="str">
-        <f>IF(H13="","",SUM(D30:AC30))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K13" s="2" t="s">
@@ -1156,16 +1152,16 @@
     <row r="14" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" t="str">
-        <f>IF(C14="","",A46)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" t="str">
-        <f>IF(H14="","",SUM(D31:AC31))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K14" s="2"/>
@@ -1177,16 +1173,16 @@
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" t="str">
-        <f>IF(C15="","",A47)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" t="str">
-        <f>IF(H15="","",SUM(D32:AC32))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K15" s="2"/>
@@ -1198,16 +1194,16 @@
     <row r="16" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" t="str">
-        <f>IF(C16="","",A48)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" t="str">
-        <f>IF(H16="","",SUM(D33:AC33))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K16" s="2"/>
@@ -1219,16 +1215,16 @@
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" t="str">
-        <f>IF(C17="","",A49)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" t="str">
-        <f>IF(H17="","",SUM(D34:AC34))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K17" s="2"/>
@@ -1240,16 +1236,16 @@
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" t="str">
-        <f>IF(C18="","",A50)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" t="str">
-        <f>IF(H18="","",SUM(D35:AC35))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K18" s="2"/>
@@ -1261,16 +1257,16 @@
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" t="str">
-        <f>IF(C19="","",A51)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" t="str">
-        <f>IF(H19="","",SUM(D36:AC36))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K19" s="2"/>
@@ -1428,7 +1424,7 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="9" t="str">
-        <f>IF(H7="","",H7)</f>
+        <f t="shared" ref="C24:C36" si="5">IF(H7="","",H7)</f>
         <v>Clase A</v>
       </c>
       <c r="D24" s="21">
@@ -1493,7 +1489,7 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="10" t="str">
-        <f>IF(H8="","",H8)</f>
+        <f t="shared" si="5"/>
         <v>Clase B</v>
       </c>
       <c r="D25" s="22">
@@ -1553,12 +1549,12 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f t="shared" ref="A26:A36" si="3">A25+1</f>
+        <f t="shared" ref="A26:A36" si="6">A25+1</f>
         <v>3</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="10" t="str">
-        <f>IF(H9="","",H9)</f>
+        <f t="shared" si="5"/>
         <v>Clase C</v>
       </c>
       <c r="D26" s="22">
@@ -1616,12 +1612,12 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="10" t="str">
-        <f>IF(H10="","",H10)</f>
+        <f t="shared" si="5"/>
         <v>Clase D</v>
       </c>
       <c r="D27" s="22">
@@ -1679,14 +1675,11 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="10" t="str">
-        <f>IF(H11="","",H11)</f>
-        <v/>
-      </c>
+      <c r="C28" s="10"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -1716,12 +1709,12 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="10" t="str">
-        <f>IF(H12="","",H12)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D29" s="15"/>
@@ -1753,12 +1746,12 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="10" t="str">
-        <f>IF(H13="","",H13)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D30" s="15"/>
@@ -1790,12 +1783,12 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="10" t="str">
-        <f>IF(H14="","",H14)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D31" s="15"/>
@@ -1827,12 +1820,12 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="10" t="str">
-        <f>IF(H15="","",H15)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D32" s="15"/>
@@ -1864,12 +1857,12 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="10" t="str">
-        <f>IF(H16="","",H16)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D33" s="15"/>
@@ -1901,12 +1894,12 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="10" t="str">
-        <f>IF(H17="","",H17)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D34" s="15"/>
@@ -1938,12 +1931,12 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="10" t="str">
-        <f>IF(H18="","",H18)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D35" s="15"/>
@@ -1975,12 +1968,12 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="27" t="str">
-        <f>IF(H19="","",H19)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="D36" s="16"/>
@@ -2012,7 +2005,7 @@
     </row>
     <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="D38">
-        <f>SUM(D24:D27)</f>
+        <f>SUM(D24:D28)</f>
         <v>16</v>
       </c>
       <c r="E38">
@@ -2020,99 +2013,99 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" ref="F38:AC38" si="4">SUM(F24:F27)</f>
+        <f t="shared" ref="F38:AC38" si="7">SUM(F24:F27)</f>
         <v>15</v>
       </c>
       <c r="G38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H38" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="K38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="M38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="O38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2130,1471 +2123,1471 @@
         <v>9</v>
       </c>
       <c r="E39" s="9">
-        <f t="shared" ref="E39:AC39" si="5">SUMIFS(E$24:E$27,F$24:F$27,$C39)</f>
+        <f t="shared" ref="E39:AC39" si="8">SUMIFS(E$24:E$27,F$24:F$27,$C39)</f>
         <v>0</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="O39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC39" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" ref="A40:A51" si="6">SUM(C40:AB40)</f>
+        <f t="shared" ref="A40:A51" si="9">SUM(C40:AB40)</f>
         <v>28</v>
       </c>
       <c r="C40" s="10" t="str">
-        <f t="shared" ref="C40:C51" si="7">C8</f>
+        <f t="shared" ref="C40:C51" si="10">C8</f>
         <v>PEPA</v>
       </c>
       <c r="D40" s="10">
-        <f t="shared" ref="D40:AC40" si="8">SUMIFS(D$24:D$27,E$24:E$27,$C40)</f>
+        <f t="shared" ref="D40:AC40" si="11">SUMIFS(D$24:D$27,E$24:E$27,$C40)</f>
         <v>0</v>
       </c>
       <c r="E40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="G40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="K40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="M40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="Q40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Z40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AC40" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="C41" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MARIO</v>
       </c>
       <c r="D41" s="10">
-        <f t="shared" ref="D41:AC41" si="9">SUMIFS(D$24:D$27,E$24:E$27,$C41)</f>
+        <f t="shared" ref="D41:AC41" si="12">SUMIFS(D$24:D$27,E$24:E$27,$C41)</f>
         <v>0</v>
       </c>
       <c r="E41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="H41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="K41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="Q41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="V41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Z41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AA41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AB41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AC41" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="C42" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>MARIA</v>
       </c>
       <c r="D42" s="10">
-        <f t="shared" ref="D42:AC42" si="10">SUMIFS(D$24:D$27,E$24:E$27,$C42)</f>
+        <f t="shared" ref="D42:AC42" si="13">SUMIFS(D$24:D$27,E$24:E$27,$C42)</f>
         <v>7</v>
       </c>
       <c r="E42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="I42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="M42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="O42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="S42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="W42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="X42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Y42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Z42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AA42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AC42" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C43" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <f t="shared" ref="D43:AC43" si="11">SUMIFS(D$24:D$27,E$24:E$27,$C43)</f>
+        <f t="shared" ref="D43:AC43" si="14">SUMIFS(D$24:D$27,E$24:E$27,$C43)</f>
         <v>0</v>
       </c>
       <c r="E43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="V43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AA43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AB43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC43" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C44" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <f t="shared" ref="D44:AC44" si="12">SUMIFS(D$24:D$27,E$24:E$27,$C44)</f>
+        <f t="shared" ref="D44:AC44" si="15">SUMIFS(D$24:D$27,E$24:E$27,$C44)</f>
         <v>0</v>
       </c>
       <c r="E44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="S44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="T44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="U44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Z44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AA44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AC44" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C45" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <f t="shared" ref="D45:AC45" si="13">SUMIFS(D$24:D$27,E$24:E$27,$C45)</f>
+        <f t="shared" ref="D45:AC45" si="16">SUMIFS(D$24:D$27,E$24:E$27,$C45)</f>
         <v>0</v>
       </c>
       <c r="E45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="T45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="V45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Y45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Z45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AB45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC45" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C46" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <f t="shared" ref="D46:AC46" si="14">SUMIFS(D$24:D$27,E$24:E$27,$C46)</f>
+        <f t="shared" ref="D46:AC46" si="17">SUMIFS(D$24:D$27,E$24:E$27,$C46)</f>
         <v>0</v>
       </c>
       <c r="E46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="V46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Z46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AA46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AB46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AC46" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C47" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <f t="shared" ref="D47:AC47" si="15">SUMIFS(D$24:D$27,E$24:E$27,$C47)</f>
+        <f t="shared" ref="D47:AC47" si="18">SUMIFS(D$24:D$27,E$24:E$27,$C47)</f>
         <v>0</v>
       </c>
       <c r="E47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="F47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="G47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="R47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="S47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="T47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="V47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="X47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Y47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AA47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AB47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AC47" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C48" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <f t="shared" ref="D48:AC48" si="16">SUMIFS(D$24:D$27,E$24:E$27,$C48)</f>
+        <f t="shared" ref="D48:AC48" si="19">SUMIFS(D$24:D$27,E$24:E$27,$C48)</f>
         <v>0</v>
       </c>
       <c r="E48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="P48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="S48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="T48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="U48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C49" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <f t="shared" ref="D49:AC49" si="17">SUMIFS(D$24:D$27,E$24:E$27,$C49)</f>
+        <f t="shared" ref="D49:AC49" si="20">SUMIFS(D$24:D$27,E$24:E$27,$C49)</f>
         <v>0</v>
       </c>
       <c r="E49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="I49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="T49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="U49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="V49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AC49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C50" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <f t="shared" ref="D50:AC50" si="18">SUMIFS(D$24:D$27,E$24:E$27,$C50)</f>
+        <f t="shared" ref="D50:AC50" si="21">SUMIFS(D$24:D$27,E$24:E$27,$C50)</f>
         <v>0</v>
       </c>
       <c r="E50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="I50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="J50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="P50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="R50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="T50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="U50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="V50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="X50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Y50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Z50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AA50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AB50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AC50" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C51" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D51" s="11">
-        <f t="shared" ref="D51:AC51" si="19">SUMIFS(D$24:D$27,E$24:E$27,$C51)</f>
+        <f t="shared" ref="D51:AC51" si="22">SUMIFS(D$24:D$27,E$24:E$27,$C51)</f>
         <v>0</v>
       </c>
       <c r="E51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="P51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Q51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="R51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="S51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="U51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="V51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="X51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Y51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Z51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AA51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AB51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AC51" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3637,19 +3630,19 @@
         <v>6</v>
       </c>
       <c r="E53" s="30">
-        <f t="shared" ref="E53:H53" si="20">IF(E72="",E$90-E$89,0)</f>
+        <f t="shared" ref="E53:H53" si="23">IF(E72="",E$90-E$89,0)</f>
         <v>0</v>
       </c>
       <c r="F53" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="G53" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="H53" s="30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="I53" s="10"/>
@@ -3676,7 +3669,7 @@
     </row>
     <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C54" s="10" t="str">
-        <f t="shared" ref="C54:C65" si="21">C40</f>
+        <f t="shared" ref="C54:C65" si="24">C40</f>
         <v>PEPA</v>
       </c>
       <c r="D54" s="28">
@@ -3684,19 +3677,19 @@
         <v>6</v>
       </c>
       <c r="E54" s="28">
-        <f t="shared" ref="E54:H54" si="22">IF(E73="",E$90-E$89,0)</f>
+        <f t="shared" ref="E54:H54" si="25">IF(E73="",E$90-E$89,0)</f>
         <v>6</v>
       </c>
       <c r="F54" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="G54" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="H54" s="28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>5</v>
       </c>
       <c r="I54" s="10"/>
@@ -3723,7 +3716,7 @@
     </row>
     <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C55" s="10" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>MARIO</v>
       </c>
       <c r="D55" s="28">
@@ -3731,19 +3724,19 @@
         <v>0</v>
       </c>
       <c r="E55" s="28">
-        <f t="shared" ref="E55:H55" si="23">IF(E74="",E$90-E$89,0)</f>
+        <f t="shared" ref="E55:H55" si="26">IF(E74="",E$90-E$89,0)</f>
         <v>6</v>
       </c>
       <c r="F55" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>6</v>
       </c>
       <c r="G55" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>6</v>
       </c>
       <c r="H55" s="28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>5</v>
       </c>
       <c r="I55" s="10"/>
@@ -3770,7 +3763,7 @@
     </row>
     <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C56" s="10" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>MARIA</v>
       </c>
       <c r="D56" s="28">
@@ -3778,19 +3771,19 @@
         <v>6</v>
       </c>
       <c r="E56" s="28">
-        <f t="shared" ref="E56:H56" si="24">IF(E75="",E$90-E$89,0)</f>
+        <f t="shared" ref="E56:H56" si="27">IF(E75="",E$90-E$89,0)</f>
         <v>0</v>
       </c>
       <c r="F56" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>6</v>
       </c>
       <c r="G56" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>6</v>
       </c>
       <c r="H56" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I56" s="10"/>
@@ -3817,27 +3810,27 @@
     </row>
     <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C57" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D57" s="28">
-        <f t="shared" ref="D57:H57" si="25">IF(D76="",D$90-D$89,0)</f>
+        <f t="shared" ref="D57:H57" si="28">IF(D76="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E57" s="28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>6</v>
       </c>
       <c r="F57" s="28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>6</v>
       </c>
       <c r="G57" s="28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>6</v>
       </c>
       <c r="H57" s="28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
       <c r="I57" s="10"/>
@@ -3864,27 +3857,27 @@
     </row>
     <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C58" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D58" s="28">
-        <f t="shared" ref="D58:H58" si="26">IF(D77="",D$90-D$89,0)</f>
+        <f t="shared" ref="D58:H58" si="29">IF(D77="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E58" s="28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="F58" s="28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="G58" s="28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="H58" s="28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>5</v>
       </c>
       <c r="I58" s="10"/>
@@ -3911,27 +3904,27 @@
     </row>
     <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C59" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D59" s="28">
-        <f t="shared" ref="D59:H59" si="27">IF(D78="",D$90-D$89,0)</f>
+        <f t="shared" ref="D59:H59" si="30">IF(D78="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E59" s="28">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="F59" s="28">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="G59" s="28">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="H59" s="28">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
       <c r="I59" s="10"/>
@@ -3958,27 +3951,27 @@
     </row>
     <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C60" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D60" s="28">
-        <f t="shared" ref="D60:H60" si="28">IF(D79="",D$90-D$89,0)</f>
+        <f t="shared" ref="D60:H60" si="31">IF(D79="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E60" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="F60" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="G60" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="H60" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="I60" s="10"/>
@@ -4005,27 +3998,27 @@
     </row>
     <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D61" s="28">
-        <f t="shared" ref="D61:H61" si="29">IF(D80="",D$90-D$89,0)</f>
+        <f t="shared" ref="D61:H61" si="32">IF(D80="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E61" s="28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="F61" s="28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="G61" s="28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="H61" s="28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="I61" s="10"/>
@@ -4052,27 +4045,27 @@
     </row>
     <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D62" s="28">
-        <f t="shared" ref="D62:H62" si="30">IF(D81="",D$90-D$89,0)</f>
+        <f t="shared" ref="D62:H62" si="33">IF(D81="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E62" s="28">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="F62" s="28">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="G62" s="28">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="H62" s="28">
-        <f t="shared" si="30"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="I62" s="10"/>
@@ -4099,27 +4092,27 @@
     </row>
     <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D63" s="28">
-        <f t="shared" ref="D63:H63" si="31">IF(D82="",D$90-D$89,0)</f>
+        <f t="shared" ref="D63:H63" si="34">IF(D82="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E63" s="28">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="F63" s="28">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="G63" s="28">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="H63" s="28">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="I63" s="10"/>
@@ -4146,27 +4139,27 @@
     </row>
     <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D64" s="28">
-        <f t="shared" ref="D64:H64" si="32">IF(D83="",D$90-D$89,0)</f>
+        <f t="shared" ref="D64:H64" si="35">IF(D83="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E64" s="28">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F64" s="28">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="G64" s="28">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="H64" s="28">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="I64" s="10"/>
@@ -4193,27 +4186,27 @@
     </row>
     <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="C65" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D65" s="27">
-        <f t="shared" ref="D65:H65" si="33">IF(D84="",D$90-D$89,0)</f>
+        <f t="shared" ref="D65:H65" si="36">IF(D84="",D$90-D$89,0)</f>
         <v>6</v>
       </c>
       <c r="E65" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="F65" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="G65" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="H65" s="27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="I65" s="10"/>
@@ -4382,7 +4375,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="9" t="str">
-        <f>IF(C7="","",C7)</f>
+        <f t="shared" ref="C72:C84" si="37">IF(C7="","",C7)</f>
         <v>PEPE</v>
       </c>
       <c r="D72" s="14"/>
@@ -4399,7 +4392,7 @@
         <v>2</v>
       </c>
       <c r="C73" s="10" t="str">
-        <f>IF(C8="","",C8)</f>
+        <f t="shared" si="37"/>
         <v>PEPA</v>
       </c>
       <c r="D73" s="15"/>
@@ -4410,11 +4403,11 @@
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" ref="A74:A84" si="34">A73+1</f>
+        <f t="shared" ref="A74:A84" si="38">A73+1</f>
         <v>3</v>
       </c>
       <c r="C74" s="10" t="str">
-        <f>IF(C9="","",C9)</f>
+        <f t="shared" si="37"/>
         <v>MARIO</v>
       </c>
       <c r="D74" s="15" t="s">
@@ -4427,11 +4420,11 @@
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="C75" s="10" t="str">
-        <f>IF(C10="","",C10)</f>
+        <f t="shared" si="37"/>
         <v>MARIA</v>
       </c>
       <c r="D75" s="15"/>
@@ -4446,11 +4439,11 @@
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>5</v>
       </c>
       <c r="C76" s="10" t="str">
-        <f>IF(C11="","",C11)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D76" s="22"/>
@@ -4461,11 +4454,11 @@
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>6</v>
       </c>
       <c r="C77" s="10" t="str">
-        <f>IF(C12="","",C12)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D77" s="22"/>
@@ -4476,11 +4469,11 @@
     </row>
     <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="C78" s="10" t="str">
-        <f>IF(C13="","",C13)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D78" s="22"/>
@@ -4491,11 +4484,11 @@
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="C79" s="10" t="str">
-        <f>IF(C14="","",C14)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D79" s="22"/>
@@ -4506,11 +4499,11 @@
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>9</v>
       </c>
       <c r="C80" s="10" t="str">
-        <f>IF(C15="","",C15)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D80" s="22"/>
@@ -4521,11 +4514,11 @@
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>10</v>
       </c>
       <c r="C81" s="10" t="str">
-        <f>IF(C16="","",C16)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D81" s="22"/>
@@ -4536,11 +4529,11 @@
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>11</v>
       </c>
       <c r="C82" s="10" t="str">
-        <f>IF(C17="","",C17)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D82" s="22"/>
@@ -4551,11 +4544,11 @@
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>12</v>
       </c>
       <c r="C83" s="28" t="str">
-        <f>IF(C18="","",C18)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D83" s="22"/>
@@ -4566,11 +4559,11 @@
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>13</v>
       </c>
       <c r="C84" s="27" t="str">
-        <f>IF(C19="","",C19)</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="D84" s="26"/>
@@ -4688,7 +4681,7 @@
       <formula>$A72&gt;$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC24:AC36 G24:G36 AA24:AA36 Y24:Y36 W24:W36 U24:U36 S24:S36 M24:M36 E24:E36 O24:O36 Q24:Q36 I24:I36 K24:K36" xr:uid="{BD0261D8-304A-4349-A29B-DD9F01694367}">
       <formula1>$C$7:$C$19</formula1>
     </dataValidation>
@@ -4702,8 +4695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EB3AAE-5DDA-4DF4-ADDC-FDC4D40DF7A1}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5259,9 +5252,9 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+      <c r="A6">
         <f>Sheet1!C28</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="B6">
         <f>Sheet1!D28</f>
@@ -6258,7 +6251,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6636,7 +6629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7204B1-4412-4601-A7E6-1F14C0007A15}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Funciones del archivo inputs.py
</commit_message>
<xml_diff>
--- a/datos/Generador inputs horarios.xlsx
+++ b/datos/Generador inputs horarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\practicaevol\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241BF4DD-2AEA-4BE9-A30A-788AA5DADD26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A3F85A-D8BF-4F4D-BB47-D9DB25C86C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,32 +50,24 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -90,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>PEPE</t>
   </si>
@@ -767,11 +759,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView showGridLines="0" topLeftCell="F13" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
@@ -1584,7 +1576,9 @@
       <c r="L26" s="22">
         <v>0</v>
       </c>
-      <c r="M26" s="22"/>
+      <c r="M26" s="22" t="s">
+        <v>3</v>
+      </c>
       <c r="N26" s="22">
         <v>3</v>
       </c>
@@ -1647,7 +1641,9 @@
       <c r="L27" s="22">
         <v>0</v>
       </c>
-      <c r="M27" s="22"/>
+      <c r="M27" s="22" t="s">
+        <v>3</v>
+      </c>
       <c r="N27" s="22">
         <v>3</v>
       </c>
@@ -4379,8 +4375,8 @@
         <v>PEPE</v>
       </c>
       <c r="D72" s="14"/>
-      <c r="E72" s="14" t="s">
-        <v>30</v>
+      <c r="E72" s="14">
+        <v>1</v>
       </c>
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
@@ -4410,8 +4406,8 @@
         <f t="shared" si="37"/>
         <v>MARIO</v>
       </c>
-      <c r="D74" s="15" t="s">
-        <v>30</v>
+      <c r="D74" s="15">
+        <v>4</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
@@ -4428,13 +4424,13 @@
         <v>MARIA</v>
       </c>
       <c r="D75" s="15"/>
-      <c r="E75" s="15" t="s">
-        <v>30</v>
+      <c r="E75" s="15">
+        <v>2</v>
       </c>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="15" t="s">
-        <v>30</v>
+      <c r="H75" s="15">
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.25">
@@ -4681,7 +4677,7 @@
       <formula>$A72&gt;$O$6</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC24:AC36 G24:G36 AA24:AA36 Y24:Y36 W24:W36 U24:U36 S24:S36 M24:M36 E24:E36 O24:O36 Q24:Q36 I24:I36 K24:K36" xr:uid="{BD0261D8-304A-4349-A29B-DD9F01694367}">
       <formula1>$C$7:$C$19</formula1>
     </dataValidation>
@@ -4696,10 +4692,10 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -5072,9 +5068,9 @@
         <f>Sheet1!L26</f>
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="str">
         <f>Sheet1!M26</f>
-        <v>0</v>
+        <v>MARIA</v>
       </c>
       <c r="L4">
         <f>Sheet1!N26</f>
@@ -5182,9 +5178,9 @@
         <f>Sheet1!L27</f>
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="str">
         <f>Sheet1!M27</f>
-        <v>0</v>
+        <v>MARIA</v>
       </c>
       <c r="L5">
         <f>Sheet1!N27</f>
@@ -5252,10 +5248,6 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>Sheet1!C28</f>
-        <v>0</v>
-      </c>
       <c r="B6">
         <f>Sheet1!D28</f>
         <v>0</v>
@@ -6251,10 +6243,10 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -6291,9 +6283,9 @@
         <f>Sheet1!D72</f>
         <v>0</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2">
         <f>Sheet1!E72</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>Sheet1!F72</f>
@@ -6339,9 +6331,9 @@
         <f>Sheet1!C74</f>
         <v>MARIO</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4">
         <f>Sheet1!D74</f>
-        <v>X</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <f>Sheet1!E74</f>
@@ -6369,9 +6361,9 @@
         <f>Sheet1!D75</f>
         <v>0</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5">
         <f>Sheet1!E75</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <f>Sheet1!F75</f>
@@ -6381,9 +6373,9 @@
         <f>Sheet1!G75</f>
         <v>0</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5">
         <f>Sheet1!H75</f>
-        <v>X</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6633,7 +6625,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">

</xml_diff>

<commit_message>
Hacer que DPF tome el valor cero en todas las horas del día si no disponible
</commit_message>
<xml_diff>
--- a/datos/Generador inputs horarios.xlsx
+++ b/datos/Generador inputs horarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\practicaevol\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A3F85A-D8BF-4F4D-BB47-D9DB25C86C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624011FE-82C0-43E3-9AC6-E7145066F557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,24 +50,32 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -759,11 +767,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F13" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
@@ -4691,11 +4699,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EB3AAE-5DDA-4DF4-ADDC-FDC4D40DF7A1}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -6246,7 +6254,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -6625,7 +6633,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">

</xml_diff>

<commit_message>
Empezado lógica para inicializar población
</commit_message>
<xml_diff>
--- a/datos/Generador inputs horarios.xlsx
+++ b/datos/Generador inputs horarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\practicaevol\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624011FE-82C0-43E3-9AC6-E7145066F557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094A0CF0-8749-4FDC-AACF-733E57F1CD98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,8 +229,17 @@
     <t>Horas totales</t>
   </si>
   <si>
+    <t>n horas asignadas</t>
+  </si>
+  <si>
+    <t>n horas disponibles</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">2. Disponibilidad profesor (marcar con una </t>
+      <t xml:space="preserve">2. Disponibilidad profesor (marcar con un </t>
     </r>
     <r>
       <rPr>
@@ -239,7 +248,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">X </t>
+      <t xml:space="preserve">1 </t>
     </r>
     <r>
       <rPr>
@@ -252,15 +261,6 @@
       </rPr>
       <t>los días no disponibles)</t>
     </r>
-  </si>
-  <si>
-    <t>n horas asignadas</t>
-  </si>
-  <si>
-    <t>n horas disponibles</t>
-  </si>
-  <si>
-    <t>Check</t>
   </si>
 </sst>
 </file>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,13 +922,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="31" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>39</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>5</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -4415,7 +4415,7 @@
         <v>MARIO</v>
       </c>
       <c r="D74" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
@@ -4433,12 +4433,12 @@
       </c>
       <c r="D75" s="15"/>
       <c r="E75" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.25">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="B4">
         <f>Sheet1!D74</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f>Sheet1!E74</f>
@@ -6371,7 +6371,7 @@
       </c>
       <c r="C5">
         <f>Sheet1!E75</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f>Sheet1!F75</f>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="F5">
         <f>Sheet1!H75</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>